<commit_message>
Include BSNE data as output, remove one bad data point
Removed bad data point on May 15 (BSNE was too low)
</commit_message>
<xml_diff>
--- a/Metadata/WeightBSNE_Oceano.xlsx
+++ b/Metadata/WeightBSNE_Oceano.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14240" tabRatio="500"/>
@@ -1981,8 +1981,8 @@
   <dimension ref="A1:P361"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3:G361"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3696,7 +3696,7 @@
         <v>2.54</v>
       </c>
       <c r="N34" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O34" s="17">
         <v>0.79305555555555562</v>

</xml_diff>